<commit_message>
Final tweaks before demo
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>Make presentation</t>
+  </si>
+  <si>
+    <t>Play with encryption</t>
+  </si>
+  <si>
+    <t>Final encryption tweaks for demo</t>
   </si>
 </sst>
 </file>
@@ -1200,11 +1206,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,6 +1780,34 @@
         <v>120</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>42612</v>
+      </c>
+      <c r="B43" s="23">
+        <v>1</v>
+      </c>
+      <c r="C43" s="23">
+        <v>27</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>42613</v>
+      </c>
+      <c r="B44" s="23">
+        <v>2</v>
+      </c>
+      <c r="C44" s="23">
+        <v>27</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1786,7 +1820,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,12 +2604,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C28" s="23">
         <f t="shared" si="0"/>
@@ -2588,15 +2622,15 @@
         <v>3</v>
       </c>
       <c r="F28" s="23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G28" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 1 Tasks'!C28)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4906,9 +4940,7 @@
   </sheetData>
   <autoFilter ref="A1:H302">
     <filterColumn colId="1">
-      <filters blank="1">
-        <filter val="In Progress"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5004,45 +5036,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>37.5</v>
+        <v>40.5</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>0.88235294117647056</v>
+        <v>0.95294117647058818</v>
       </c>
       <c r="K2" s="16">
         <v>42527</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42610</v>
+        <v>42613</v>
       </c>
       <c r="M2" s="16">
         <v>42580</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>-30</v>
+        <v>-33</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>1.5660377358490567</v>
+        <v>1.6226415094339623</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.68368479467258614</v>
+        <v>-0.66970033296337417</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-36.235294117647065</v>
+        <v>-35.494117647058829</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5119,15 +5151,15 @@
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 1 Tasks'!G:G,'Phase 1 Tasks'!D:D,A7)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
         <f>SUMIFS('Phase 1 Tasks'!F:F,'Phase 1 Tasks'!D:D,A7)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>0.76923076923076927</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -9828,30 +9860,30 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42610</v>
+        <v>42613</v>
       </c>
       <c r="M2" s="16">
         <v>42647</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>0.13953488372093023</v>
+        <v>0.20930232558139536</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.12258573117855735</v>
+        <v>-0.19235317303902247</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-5.2711864406779663</v>
+        <v>-8.2711864406779654</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -14638,18 +14670,18 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42610</v>
+        <v>42613</v>
       </c>
       <c r="M2" s="16">
         <v>42713</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>-37</v>
+        <v>-34</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">IF(N2&gt;0,N2/(N2+O2),0)</f>
@@ -16560,47 +16592,47 @@
       </c>
       <c r="N2" s="17">
         <f ca="1">TODAY()</f>
-        <v>42610</v>
+        <v>42613</v>
       </c>
       <c r="O2" s="17">
         <v>42713</v>
       </c>
       <c r="P2" s="5">
         <f ca="1">N2-M2</f>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="5">
         <v>25</v>
       </c>
       <c r="R2" s="5">
         <f ca="1">O2-N2</f>
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S2" s="28">
         <f ca="1">IF(P2&gt;0,(P2-Q2)/(P2+R2-Q2),0)</f>
-        <v>0.36024844720496896</v>
+        <v>0.37888198757763975</v>
       </c>
       <c r="T2" s="6">
         <f ca="1">G10-S2</f>
-        <v>-0.11580400276052452</v>
+        <v>-0.11538992408557625</v>
       </c>
       <c r="U2" s="30">
         <f ca="1">T2*(P2+R2-Q2)</f>
-        <v>-18.644444444444449</v>
+        <v>-18.577777777777776</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <f>'Phase 1 Portfolio'!G2</f>
-        <v>37.5</v>
+        <v>40.5</v>
       </c>
       <c r="B3" s="32">
         <f>'Phase 1 Portfolio'!H2</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="33">
         <f>'Phase 1 Portfolio'!I2</f>
-        <v>0.88235294117647056</v>
+        <v>0.95294117647058818</v>
       </c>
       <c r="E3" s="31">
         <f>'Phase 2 Portfolio'!G2</f>
@@ -16649,15 +16681,15 @@
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="31">
         <f>A3+E3+I3</f>
-        <v>38.5</v>
+        <v>41.5</v>
       </c>
       <c r="F10" s="32">
         <f>B3+F3+J3</f>
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G10" s="33">
         <f>E10/(E10+F10)</f>
-        <v>0.24444444444444444</v>
+        <v>0.2634920634920635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorg for Phase two and Formal Specification
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Time Log" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Phase 1 Tasks'!$A$1:$H$302</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase 2 Tasks'!$A$1:$H$302</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase 2 Tasks'!$A$1:$H$303</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Phase 3 Tasks'!$A$1:$H$302</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="133">
   <si>
     <t>Date</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Set Up Vision Doc</t>
@@ -323,9 +320,6 @@
     <t>Revise Project Plan</t>
   </si>
   <si>
-    <t>Create Formal Specification</t>
-  </si>
-  <si>
     <t>Formal Specification</t>
   </si>
   <si>
@@ -405,6 +399,42 @@
   </si>
   <si>
     <t>Final encryption tweaks for demo</t>
+  </si>
+  <si>
+    <t>Email about feedback</t>
+  </si>
+  <si>
+    <t>Review Possilbe Revisions</t>
+  </si>
+  <si>
+    <t>Set Up Formal Spec</t>
+  </si>
+  <si>
+    <t>Set up and look at Use</t>
+  </si>
+  <si>
+    <t>Set Up Classes</t>
+  </si>
+  <si>
+    <t>Set Up Associations</t>
+  </si>
+  <si>
+    <t>Set Up Constraints</t>
+  </si>
+  <si>
+    <t>Working on Classes</t>
+  </si>
+  <si>
+    <t>Finishing up classes</t>
+  </si>
+  <si>
+    <t>Finish Associations</t>
+  </si>
+  <si>
+    <t>Decide on Constraints</t>
+  </si>
+  <si>
+    <t>Finish Constraints</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1236,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1305,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1319,7 +1349,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1333,7 +1363,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,7 +1377,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1361,7 +1391,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,7 +1405,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,7 +1433,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1417,7 +1447,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1431,7 +1461,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1445,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,7 +1531,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1529,7 +1559,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,7 +1573,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,7 +1601,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1599,7 +1629,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1613,7 +1643,7 @@
         <v>16</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1641,7 +1671,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1655,7 +1685,7 @@
         <v>22</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1735,7 +1765,7 @@
         <v>26</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1749,7 +1779,7 @@
         <v>26</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1763,7 +1793,7 @@
         <v>30</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,7 +1807,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1791,7 +1821,7 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1805,7 +1835,141 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
+        <v>42614</v>
+      </c>
+      <c r="B45" s="23">
+        <v>1</v>
+      </c>
+      <c r="C45" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
+        <v>42614</v>
+      </c>
+      <c r="B46" s="23">
+        <v>1</v>
+      </c>
+      <c r="C46" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="17">
+        <v>42618</v>
+      </c>
+      <c r="B47" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="23">
+        <v>31</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="17">
+        <v>42626</v>
+      </c>
+      <c r="B48" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="23">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
+        <v>42626</v>
+      </c>
+      <c r="B49" s="23">
+        <v>1</v>
+      </c>
+      <c r="C49" s="23">
+        <v>42</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>42631</v>
+      </c>
+      <c r="B50" s="23">
+        <v>1</v>
+      </c>
+      <c r="C50" s="23">
+        <v>43</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
+        <v>42632</v>
+      </c>
+      <c r="B51" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C51" s="23">
+        <v>43</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <v>42632</v>
+      </c>
+      <c r="B52" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="23">
+        <v>44</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
+        <v>42632</v>
+      </c>
+      <c r="B53" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C53" s="23">
+        <v>33</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
+        <v>42633</v>
+      </c>
+      <c r="B54" s="23">
+        <v>1</v>
+      </c>
+      <c r="C54" s="23">
+        <v>33</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1815,12 +1979,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,12 +2023,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="21">
         <v>1</v>
@@ -1888,12 +2051,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C34" si="0">C2+1</f>
@@ -1917,12 +2080,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="0"/>
@@ -1946,12 +2109,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="0"/>
@@ -1975,12 +2138,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
@@ -2006,7 +2169,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
@@ -2019,23 +2185,23 @@
         <v>1</v>
       </c>
       <c r="F7" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 1 Tasks'!C7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
@@ -2059,12 +2225,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
@@ -2088,12 +2254,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" si="0"/>
@@ -2117,12 +2283,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" si="0"/>
@@ -2146,12 +2312,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="23">
         <f t="shared" si="0"/>
@@ -2175,12 +2341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
@@ -2204,12 +2370,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="23">
         <f t="shared" si="0"/>
@@ -2233,12 +2399,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="23">
         <f t="shared" si="0"/>
@@ -2262,12 +2428,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="23">
         <f t="shared" si="0"/>
@@ -2291,12 +2457,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="23">
         <f t="shared" si="0"/>
@@ -2320,12 +2486,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="23">
         <f t="shared" si="0"/>
@@ -2346,12 +2512,12 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="23">
         <f t="shared" si="0"/>
@@ -2375,12 +2541,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="23">
         <f t="shared" si="0"/>
@@ -2404,12 +2570,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="23">
         <f t="shared" si="0"/>
@@ -2433,12 +2599,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="23">
         <f t="shared" si="0"/>
@@ -2462,12 +2628,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="23">
         <f t="shared" si="0"/>
@@ -2491,12 +2657,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="23">
         <f t="shared" si="0"/>
@@ -2520,12 +2686,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="23">
         <f t="shared" si="0"/>
@@ -2551,7 +2717,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C26" s="23">
         <f t="shared" si="0"/>
@@ -2564,23 +2733,23 @@
         <v>1</v>
       </c>
       <c r="F26" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 1 Tasks'!C26)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="23">
         <f t="shared" si="0"/>
@@ -2604,12 +2773,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="23">
         <f t="shared" si="0"/>
@@ -4938,11 +5107,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H302">
-    <filterColumn colId="1">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H302"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -4954,7 +5119,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4994,28 +5159,28 @@
         <v>13</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -5036,45 +5201,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>40.5</v>
+        <v>42.5</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>0.95294117647058818</v>
+        <v>1</v>
       </c>
       <c r="K2" s="16">
         <v>42527</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42613</v>
+        <v>42633</v>
       </c>
       <c r="M2" s="16">
         <v>42580</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="O2" s="5">
-        <f ca="1">M2-L2</f>
-        <v>-33</v>
+        <f ca="1">IF(M2-L2&gt;0,M2-L2,0)</f>
+        <v>0</v>
       </c>
       <c r="P2" s="28">
-        <f ca="1">N2/(N2+O2)</f>
-        <v>1.6226415094339623</v>
+        <f ca="1">IF(N2/(N2+O2)&gt;1,1,N2/(N2+O2))</f>
+        <v>1</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.66970033296337417</v>
+        <v>0</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-35.494117647058829</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5134,15 +5299,15 @@
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 1 Tasks'!G:G,'Phase 1 Tasks'!D:D,A6)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5">
         <f>SUMIFS('Phase 1 Tasks'!F:F,'Phase 1 Tasks'!D:D,A6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -6881,7 +7046,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6923,10 +7088,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C2" s="21">
         <v>30</v>
@@ -6951,7 +7116,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C66" si="0">C2+1</f>
@@ -6964,20 +7132,23 @@
         <v>3</v>
       </c>
       <c r="F3" s="23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C3)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="22">
         <f t="shared" ref="H3:H66" si="1">IF(F3+G3&gt;0,G3/(G3+F3),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="0"/>
@@ -6990,53 +7161,56 @@
         <v>3</v>
       </c>
       <c r="F4" s="23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C4)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>127</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E5" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C5)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H5" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="23">
         <v>5</v>
@@ -7055,14 +7229,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="23">
         <v>10</v>
@@ -7081,14 +7255,14 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="23">
         <v>2</v>
@@ -7107,14 +7281,14 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="23">
         <v>6</v>
@@ -7133,7 +7307,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" si="0"/>
@@ -7159,7 +7333,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" si="0"/>
@@ -7185,7 +7359,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="23">
         <f t="shared" si="0"/>
@@ -7211,7 +7385,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
@@ -7236,45 +7410,90 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" s="23">
         <f t="shared" si="0"/>
         <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="23">
+        <v>1</v>
+      </c>
+      <c r="F14" s="23">
+        <v>0</v>
       </c>
       <c r="G14" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C14)</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2</v>
+      </c>
+      <c r="F15" s="23">
         <v>0</v>
-      </c>
-      <c r="H14" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="23">
-        <f t="shared" si="0"/>
-        <v>43</v>
       </c>
       <c r="G15" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C15)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="23">
+        <v>1</v>
+      </c>
+      <c r="F16" s="23">
         <v>0</v>
-      </c>
-      <c r="H15" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="23">
-        <f t="shared" si="0"/>
-        <v>44</v>
       </c>
       <c r="G16" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C16)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -9751,7 +9970,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H302"/>
+  <autoFilter ref="A1:H303"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -9761,9 +9980,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9803,28 +10022,28 @@
         <v>13</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -9845,45 +10064,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>1.6949152542372881E-2</v>
+        <v>0.12149532710280374</v>
       </c>
       <c r="K2" s="16">
         <v>42604</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42613</v>
+        <v>42633</v>
       </c>
       <c r="M2" s="16">
-        <v>42647</v>
+        <v>42649</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>0.20930232558139536</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.19235317303902247</v>
+        <v>-0.52294911734164073</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-8.2711864406779654</v>
+        <v>-23.532710280373834</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -9892,15 +10111,15 @@
       </c>
       <c r="B3" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A3)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C3" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A3)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D67" si="0">IF(C3+B3&gt;0,B3/(B3+C3),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -9909,37 +10128,37 @@
       </c>
       <c r="B4" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A4)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A4)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A5)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="C5" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5" si="1">IF(C5+B5&gt;0,B5/(B5+C5),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A6)</f>
@@ -9956,7 +10175,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A7)</f>
@@ -9973,7 +10192,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A8)</f>
@@ -11771,14 +11990,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="21">
         <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" s="21">
         <v>12</v>
@@ -11797,14 +12016,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C66" si="0">C2+1</f>
         <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E3" s="23">
         <v>25</v>
@@ -11823,14 +12042,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E4" s="23">
         <v>4</v>
@@ -11849,14 +12068,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E5" s="23">
         <v>4</v>
@@ -11875,14 +12094,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E6" s="23">
         <v>6</v>
@@ -11901,14 +12120,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E7" s="23">
         <v>1</v>
@@ -11927,7 +12146,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
@@ -11953,7 +12172,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
@@ -11979,7 +12198,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" si="0"/>
@@ -14573,7 +14792,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14613,28 +14832,28 @@
         <v>13</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -14666,22 +14885,22 @@
         <v>0</v>
       </c>
       <c r="K2" s="16">
-        <v>42647</v>
+        <v>42649</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42613</v>
+        <v>42633</v>
       </c>
       <c r="M2" s="16">
         <v>42713</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>-34</v>
+        <v>-16</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">IF(N2&gt;0,N2/(N2+O2),0)</f>
@@ -14698,7 +14917,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A3)</f>
@@ -14715,7 +14934,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A4)</f>
@@ -14732,7 +14951,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A5)</f>
@@ -14749,7 +14968,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A6)</f>
@@ -14766,7 +14985,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A7)</f>
@@ -16504,7 +16723,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16517,51 +16736,51 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="E1" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
       <c r="I1" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J1" s="36"/>
       <c r="K1" s="37"/>
       <c r="M1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" s="29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -16570,7 +16789,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
@@ -16579,7 +16798,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>7</v>
@@ -16592,59 +16811,59 @@
       </c>
       <c r="N2" s="17">
         <f ca="1">TODAY()</f>
-        <v>42613</v>
+        <v>42633</v>
       </c>
       <c r="O2" s="17">
         <v>42713</v>
       </c>
       <c r="P2" s="5">
         <f ca="1">N2-M2</f>
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="Q2" s="5">
         <v>25</v>
       </c>
       <c r="R2" s="5">
         <f ca="1">O2-N2</f>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="S2" s="28">
         <f ca="1">IF(P2&gt;0,(P2-Q2)/(P2+R2-Q2),0)</f>
-        <v>0.37888198757763975</v>
+        <v>0.50310559006211175</v>
       </c>
       <c r="T2" s="6">
         <f ca="1">G10-S2</f>
-        <v>-0.11538992408557625</v>
+        <v>-0.18073716900948017</v>
       </c>
       <c r="U2" s="30">
         <f ca="1">T2*(P2+R2-Q2)</f>
-        <v>-18.577777777777776</v>
+        <v>-29.098684210526308</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <f>'Phase 1 Portfolio'!G2</f>
-        <v>40.5</v>
+        <v>42.5</v>
       </c>
       <c r="B3" s="32">
         <f>'Phase 1 Portfolio'!H2</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="33">
         <f>'Phase 1 Portfolio'!I2</f>
-        <v>0.95294117647058818</v>
+        <v>1</v>
       </c>
       <c r="E3" s="31">
         <f>'Phase 2 Portfolio'!G2</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="F3" s="32">
         <f>'Phase 2 Portfolio'!H2</f>
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="G3" s="33">
         <f>'Phase 2 Portfolio'!I2</f>
-        <v>1.6949152542372881E-2</v>
+        <v>0.12149532710280374</v>
       </c>
       <c r="I3" s="31">
         <f>'Phase 3 Portfolio'!G2</f>
@@ -16662,14 +16881,14 @@
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>7</v>
@@ -16681,15 +16900,15 @@
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="31">
         <f>A3+E3+I3</f>
-        <v>41.5</v>
+        <v>49</v>
       </c>
       <c r="F10" s="32">
         <f>B3+F3+J3</f>
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G10" s="33">
         <f>E10/(E10+F10)</f>
-        <v>0.2634920634920635</v>
+        <v>0.32236842105263158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished arch des doc
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Time Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -323,12 +323,6 @@
     <t>Formal Specification</t>
   </si>
   <si>
-    <t>Create Architectural Design</t>
-  </si>
-  <si>
-    <t>Create Test Plan</t>
-  </si>
-  <si>
     <t>Create Inspection Checklist</t>
   </si>
   <si>
@@ -435,6 +429,54 @@
   </si>
   <si>
     <t>Finish Constraints</t>
+  </si>
+  <si>
+    <t>Set Up Architectural Design</t>
+  </si>
+  <si>
+    <t>Set up document</t>
+  </si>
+  <si>
+    <t>Finish Section 2</t>
+  </si>
+  <si>
+    <t>Finish Section 3</t>
+  </si>
+  <si>
+    <t>Finish Section 4</t>
+  </si>
+  <si>
+    <t>Finish Section 5</t>
+  </si>
+  <si>
+    <t>Finish Section 1</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Finished component diagram and interface specification</t>
+  </si>
+  <si>
+    <t>Finish section 2</t>
+  </si>
+  <si>
+    <t>Finish Document</t>
+  </si>
+  <si>
+    <t>Prep for Test Plan</t>
+  </si>
+  <si>
+    <t>Set Up Document</t>
+  </si>
+  <si>
+    <t>Finish Sections 1 - 8</t>
+  </si>
+  <si>
+    <t>Finish Section 9-11</t>
+  </si>
+  <si>
+    <t>Review Test plan document structure</t>
   </si>
 </sst>
 </file>
@@ -1236,19 +1278,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="23"/>
+    <col min="1" max="1" width="12.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="23"/>
     <col min="3" max="3" width="11" style="23" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1807,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,7 +1863,7 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1877,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,7 +1913,7 @@
         <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,7 +1927,7 @@
         <v>32</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,7 +1941,7 @@
         <v>42</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,7 +1955,7 @@
         <v>43</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1969,7 @@
         <v>43</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,7 +1983,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +1997,7 @@
         <v>33</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +2011,99 @@
         <v>33</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
+        <v>42633</v>
+      </c>
+      <c r="B55" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C55" s="23">
+        <v>45</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <v>42637</v>
+      </c>
+      <c r="B56" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="C56" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
+        <v>42637</v>
+      </c>
+      <c r="B57" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C57" s="23">
+        <v>46</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="17">
+        <v>42638</v>
+      </c>
+      <c r="B58" s="23">
+        <v>1</v>
+      </c>
+      <c r="C58" s="23">
+        <v>46</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
+        <v>42638</v>
+      </c>
+      <c r="B59" s="23">
+        <v>1</v>
+      </c>
+      <c r="C59" s="23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
+        <v>42646</v>
+      </c>
+      <c r="B60" s="23">
+        <v>2</v>
+      </c>
+      <c r="C60" s="23">
+        <v>48</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
+        <v>42646</v>
+      </c>
+      <c r="B61" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C61" s="23">
+        <v>35</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1988,13 +2122,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="10.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="24" customWidth="1"/>
-    <col min="9" max="10" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="42.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="24" customWidth="1"/>
+    <col min="9" max="10" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5124,16 +5258,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="4"/>
+    <col min="5" max="6" width="4.75" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5216,14 +5350,14 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42633</v>
+        <v>42646</v>
       </c>
       <c r="M2" s="16">
         <v>42580</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">IF(M2-L2&gt;0,M2-L2,0)</f>
@@ -7044,20 +7178,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H302"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="10.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="24" customWidth="1"/>
-    <col min="9" max="10" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="42.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="24" customWidth="1"/>
+    <col min="9" max="10" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7174,7 +7308,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>38</v>
@@ -7202,34 +7336,31 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E6" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F6" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C6)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H6" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>142</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
@@ -7239,23 +7370,23 @@
         <v>88</v>
       </c>
       <c r="E7" s="23">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="23">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G7" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C7)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
@@ -7281,7 +7412,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
@@ -7291,10 +7422,10 @@
         <v>89</v>
       </c>
       <c r="E9" s="23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" s="23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C9)</f>
@@ -7307,7 +7438,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" si="0"/>
@@ -7317,10 +7448,10 @@
         <v>22</v>
       </c>
       <c r="E10" s="23">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F10" s="23">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G10" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C10)</f>
@@ -7333,7 +7464,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" si="0"/>
@@ -7343,10 +7474,10 @@
         <v>21</v>
       </c>
       <c r="E11" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C11)</f>
@@ -7369,10 +7500,10 @@
         <v>21</v>
       </c>
       <c r="E12" s="23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C12)</f>
@@ -7385,7 +7516,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
@@ -7411,7 +7542,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>38</v>
@@ -7440,7 +7571,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>38</v>
@@ -7469,7 +7600,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>38</v>
@@ -7496,66 +7627,141 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C17" s="23">
         <f t="shared" si="0"/>
         <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0</v>
       </c>
       <c r="G17" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C17)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="23">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="23">
         <v>0</v>
-      </c>
-      <c r="H17" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="23">
-        <f t="shared" si="0"/>
-        <v>46</v>
       </c>
       <c r="G18" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C18)</f>
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="23">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19" s="23">
         <v>0</v>
-      </c>
-      <c r="H18" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="23">
-        <f t="shared" si="0"/>
-        <v>47</v>
       </c>
       <c r="G19" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C19)</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="23">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20" s="23">
         <v>0</v>
-      </c>
-      <c r="H19" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="23">
-        <f t="shared" si="0"/>
-        <v>48</v>
       </c>
       <c r="G20" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C20)</f>
+        <v>2</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="23">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="23">
+        <v>1</v>
+      </c>
+      <c r="F21" s="23">
         <v>0</v>
-      </c>
-      <c r="H20" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="23">
-        <f t="shared" si="0"/>
-        <v>49</v>
       </c>
       <c r="G21" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C21)</f>
@@ -7566,64 +7772,123 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C22" s="23">
         <f t="shared" si="0"/>
         <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="F22" s="23">
+        <v>0</v>
       </c>
       <c r="G22" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C22)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="C23" s="23">
         <f t="shared" si="0"/>
         <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0.5</v>
       </c>
       <c r="G23" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C23)</f>
         <v>0</v>
       </c>
-      <c r="H23" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="C24" s="23">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="23">
+        <v>1</v>
+      </c>
+      <c r="F24" s="23">
+        <v>1</v>
+      </c>
       <c r="G24" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C24)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="22" t="str">
+      <c r="H24" s="22">
         <f>IF(F24+G24&gt;0,G24/(G24+F24),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="C25" s="23">
         <f t="shared" si="0"/>
         <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="23">
+        <v>2</v>
+      </c>
+      <c r="F25" s="23">
+        <v>2</v>
       </c>
       <c r="G25" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C25)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="23">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -7637,7 +7902,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="23">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -7651,7 +7916,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="23">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -7665,7 +7930,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="23">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -7675,7 +7940,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C30" s="23">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -7685,7 +7950,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="23">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -7695,7 +7960,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="23">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -9980,23 +10245,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="4"/>
+    <col min="5" max="6" width="4.75" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10064,45 +10329,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>6.5</v>
+        <v>13.25</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>0.12149532710280374</v>
+        <v>0.39849624060150374</v>
       </c>
       <c r="K2" s="16">
         <v>42604</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42633</v>
+        <v>42646</v>
       </c>
       <c r="M2" s="16">
-        <v>42649</v>
+        <v>42661</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>0.64444444444444449</v>
+        <v>0.73684210526315785</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.52294911734164073</v>
+        <v>-0.33834586466165412</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-23.532710280373834</v>
+        <v>-19.285714285714285</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -10162,15 +10427,15 @@
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A6)</f>
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="C6" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A6)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -10179,15 +10444,15 @@
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A7)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A7)</f>
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -10200,7 +10465,7 @@
       </c>
       <c r="C8" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A8)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
@@ -10217,7 +10482,7 @@
       </c>
       <c r="C9" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A9)</f>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
@@ -10234,7 +10499,7 @@
       </c>
       <c r="C10" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A10)</f>
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
@@ -11953,13 +12218,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="10.7109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="24" customWidth="1"/>
-    <col min="9" max="10" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="42.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="23.875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="24" customWidth="1"/>
+    <col min="9" max="10" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11990,14 +12255,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="21">
         <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E2" s="21">
         <v>12</v>
@@ -12016,14 +12281,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C66" si="0">C2+1</f>
         <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="23">
         <v>25</v>
@@ -12042,14 +12307,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="23">
         <v>4</v>
@@ -12068,14 +12333,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="23">
         <v>4</v>
@@ -12094,14 +12359,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="23">
         <v>6</v>
@@ -12120,14 +12385,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E7" s="23">
         <v>1</v>
@@ -12146,7 +12411,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
@@ -14797,16 +15062,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="4"/>
+    <col min="5" max="6" width="4.75" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14889,18 +15154,18 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42633</v>
+        <v>42646</v>
       </c>
       <c r="M2" s="16">
         <v>42713</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>-16</v>
+        <v>-3</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">IF(N2&gt;0,N2/(N2+O2),0)</f>
@@ -14917,7 +15182,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A3)</f>
@@ -14934,7 +15199,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A4)</f>
@@ -14951,7 +15216,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A5)</f>
@@ -14968,7 +15233,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A6)</f>
@@ -14985,7 +15250,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A7)</f>
@@ -16728,25 +16993,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="15" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="13" max="15" width="12.75" customWidth="1"/>
+    <col min="17" max="17" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.25" customWidth="1"/>
+    <col min="21" max="21" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="E1" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
       <c r="I1" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J1" s="36"/>
       <c r="K1" s="37"/>
@@ -16754,7 +17019,7 @@
         <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>51</v>
@@ -16763,7 +17028,7 @@
         <v>48</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>52</v>
@@ -16811,33 +17076,33 @@
       </c>
       <c r="N2" s="17">
         <f ca="1">TODAY()</f>
-        <v>42633</v>
+        <v>42646</v>
       </c>
       <c r="O2" s="17">
         <v>42713</v>
       </c>
       <c r="P2" s="5">
         <f ca="1">N2-M2</f>
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="Q2" s="5">
         <v>25</v>
       </c>
       <c r="R2" s="5">
         <f ca="1">O2-N2</f>
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="S2" s="28">
         <f ca="1">IF(P2&gt;0,(P2-Q2)/(P2+R2-Q2),0)</f>
-        <v>0.50310559006211175</v>
+        <v>0.58385093167701863</v>
       </c>
       <c r="T2" s="6">
         <f ca="1">G10-S2</f>
-        <v>-0.18073716900948017</v>
+        <v>-0.16070102655367896</v>
       </c>
       <c r="U2" s="30">
         <f ca="1">T2*(P2+R2-Q2)</f>
-        <v>-29.098684210526308</v>
+        <v>-25.872865275142313</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16855,15 +17120,15 @@
       </c>
       <c r="E3" s="31">
         <f>'Phase 2 Portfolio'!G2</f>
-        <v>6.5</v>
+        <v>13.25</v>
       </c>
       <c r="F3" s="32">
         <f>'Phase 2 Portfolio'!H2</f>
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G3" s="33">
         <f>'Phase 2 Portfolio'!I2</f>
-        <v>0.12149532710280374</v>
+        <v>0.39849624060150374</v>
       </c>
       <c r="I3" s="31">
         <f>'Phase 3 Portfolio'!G2</f>
@@ -16881,7 +17146,7 @@
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
@@ -16900,15 +17165,15 @@
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="31">
         <f>A3+E3+I3</f>
-        <v>49</v>
+        <v>55.75</v>
       </c>
       <c r="F10" s="32">
         <f>B3+F3+J3</f>
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="G10" s="33">
         <f>E10/(E10+F10)</f>
-        <v>0.32236842105263158</v>
+        <v>0.42314990512333966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished prototype and prep for presentation
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Time Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="157">
   <si>
     <t>Date</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Formal Specification</t>
   </si>
   <si>
-    <t>Create Inspection Checklist</t>
-  </si>
-  <si>
     <t>Perform Inspection</t>
   </si>
   <si>
@@ -480,6 +477,36 @@
   </si>
   <si>
     <t>Finish sections 1-8</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Finished document set up</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Set Up Presentation</t>
+  </si>
+  <si>
+    <t>Finish Presentation</t>
+  </si>
+  <si>
+    <t>Finished setup/prep</t>
+  </si>
+  <si>
+    <t>Creating Presentation</t>
+  </si>
+  <si>
+    <t>Studied up on classes and modules, build user classes</t>
+  </si>
+  <si>
+    <t>Setting up console control flow</t>
+  </si>
+  <si>
+    <t>Finish conosle code for users</t>
   </si>
 </sst>
 </file>
@@ -1281,11 +1308,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,7 +1907,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1943,7 @@
         <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,7 +1957,7 @@
         <v>32</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,7 +1971,7 @@
         <v>42</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,7 +1985,7 @@
         <v>43</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,7 +1999,7 @@
         <v>43</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +2013,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,7 +2027,7 @@
         <v>33</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2041,7 @@
         <v>33</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,7 +2055,7 @@
         <v>45</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2080,7 @@
         <v>46</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,7 +2094,7 @@
         <v>46</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +2119,7 @@
         <v>48</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,7 +2147,7 @@
         <v>51</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +2161,7 @@
         <v>52</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,6 +2176,104 @@
       </c>
       <c r="D64" s="2" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="17">
+        <v>42659</v>
+      </c>
+      <c r="B65" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="C65" s="23">
+        <v>54</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="17">
+        <v>42659</v>
+      </c>
+      <c r="B66" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C66" s="23">
+        <v>55</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="17">
+        <v>42661</v>
+      </c>
+      <c r="B67" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="C67" s="23">
+        <v>56</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="17">
+        <v>42661</v>
+      </c>
+      <c r="B68" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C68" s="23">
+        <v>57</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="17">
+        <v>42664</v>
+      </c>
+      <c r="B69" s="23">
+        <v>2</v>
+      </c>
+      <c r="C69" s="23">
+        <v>38</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17">
+        <v>42665</v>
+      </c>
+      <c r="B70" s="23">
+        <v>2</v>
+      </c>
+      <c r="C70" s="23">
+        <v>38</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17">
+        <v>42666</v>
+      </c>
+      <c r="B71" s="23">
+        <v>6</v>
+      </c>
+      <c r="C71" s="23">
+        <v>38</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5395,14 +5520,14 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42654</v>
+        <v>42666</v>
       </c>
       <c r="M2" s="16">
         <v>42580</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">IF(M2-L2&gt;0,M2-L2,0)</f>
@@ -7225,7 +7350,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7353,7 +7478,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>38</v>
@@ -7402,7 +7527,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>38</v>
@@ -7430,34 +7555,25 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
         <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="23">
-        <v>2</v>
-      </c>
-      <c r="F8" s="23">
-        <v>2</v>
       </c>
       <c r="G8" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C8)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H8" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>149</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
@@ -7467,23 +7583,26 @@
         <v>89</v>
       </c>
       <c r="E9" s="23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C9)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H9" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="23">
         <f t="shared" si="0"/>
@@ -7496,47 +7615,38 @@
         <v>8</v>
       </c>
       <c r="F10" s="23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G10" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C10)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H10" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C11" s="23">
         <f t="shared" si="0"/>
         <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="23">
-        <v>1</v>
-      </c>
-      <c r="F11" s="23">
-        <v>1</v>
       </c>
       <c r="G11" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H11" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B12" s="20" t="s">
+        <v>147</v>
+      </c>
       <c r="C12" s="23">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -7561,7 +7671,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
@@ -7587,7 +7700,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>38</v>
@@ -7616,7 +7729,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>38</v>
@@ -7645,7 +7758,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>38</v>
@@ -7674,7 +7787,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>38</v>
@@ -7703,7 +7816,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>38</v>
@@ -7732,7 +7845,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>38</v>
@@ -7761,7 +7874,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>38</v>
@@ -7790,7 +7903,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>38</v>
@@ -7819,7 +7932,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>38</v>
@@ -7848,7 +7961,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>38</v>
@@ -7877,7 +7990,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>38</v>
@@ -7906,7 +8019,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>38</v>
@@ -7934,55 +8047,119 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C26" s="23">
         <f t="shared" si="0"/>
         <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0</v>
       </c>
       <c r="G26" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C26)</f>
+        <v>0.25</v>
+      </c>
+      <c r="H26" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="23">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="23">
+        <v>1</v>
+      </c>
+      <c r="F27" s="23">
         <v>0</v>
-      </c>
-      <c r="H26" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="23">
-        <f t="shared" si="0"/>
-        <v>55</v>
       </c>
       <c r="G27" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C27)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="23">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="23">
         <v>0</v>
-      </c>
-      <c r="H27" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="23">
-        <f t="shared" si="0"/>
-        <v>56</v>
       </c>
       <c r="G28" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C28)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0.25</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>147</v>
+      </c>
       <c r="C29" s="23">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="H29" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="23">
+        <v>1</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="21">
+        <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C29)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H29" s="22">
+        <f t="shared" ref="H29:H32" si="2">IF(F29+G29&gt;0,G29/(G29+F29),"")</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -7990,8 +8167,12 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
+      <c r="G30" s="21">
+        <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C30)</f>
+        <v>0</v>
+      </c>
       <c r="H30" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8000,8 +8181,12 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
+      <c r="G31" s="21">
+        <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C31)</f>
+        <v>0</v>
+      </c>
       <c r="H31" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8010,8 +8195,12 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="G32" s="21">
+        <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 2 Tasks'!C32)</f>
+        <v>0</v>
+      </c>
       <c r="H32" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8357,1925 +8546,1925 @@
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C67" s="23">
-        <f t="shared" ref="C67:C130" si="2">C66+1</f>
+        <f t="shared" ref="C67:C130" si="3">C66+1</f>
         <v>95</v>
       </c>
       <c r="H67" s="22" t="str">
-        <f t="shared" ref="H67:H130" si="3">IF(F67+G67&gt;0,G67/(G67+F67),"")</f>
+        <f t="shared" ref="H67:H130" si="4">IF(F67+G67&gt;0,G67/(G67+F67),"")</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C68" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="H68" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C69" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="H69" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C70" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="H70" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C71" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="H71" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C72" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="H72" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C73" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="H73" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="H74" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C75" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="H75" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C76" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="H76" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C77" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="H77" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106</v>
       </c>
       <c r="H78" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>107</v>
       </c>
       <c r="H79" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C80" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108</v>
       </c>
       <c r="H80" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C81" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="H81" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C82" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="H82" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C83" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="H83" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C84" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112</v>
       </c>
       <c r="H84" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C85" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="H85" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C86" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="H86" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C87" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="H87" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C88" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="H88" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C89" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="H89" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C90" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="H90" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C91" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>119</v>
       </c>
       <c r="H91" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C92" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="H92" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C93" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="H93" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C94" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122</v>
       </c>
       <c r="H94" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C95" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123</v>
       </c>
       <c r="H95" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C96" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="H96" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C97" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="H97" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C98" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="H98" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C99" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>127</v>
       </c>
       <c r="H99" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C100" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="H100" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C101" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>129</v>
       </c>
       <c r="H101" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C102" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="H102" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C103" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="H103" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C104" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="H104" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C105" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133</v>
       </c>
       <c r="H105" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C106" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134</v>
       </c>
       <c r="H106" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C107" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135</v>
       </c>
       <c r="H107" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C108" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="H108" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C109" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>137</v>
       </c>
       <c r="H109" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C110" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="H110" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C111" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>139</v>
       </c>
       <c r="H111" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C112" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="H112" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C113" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="H113" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C114" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>142</v>
       </c>
       <c r="H114" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C115" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="H115" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C116" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144</v>
       </c>
       <c r="H116" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C117" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="H117" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C118" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="H118" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C119" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>147</v>
       </c>
       <c r="H119" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C120" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="H120" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C121" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>149</v>
       </c>
       <c r="H121" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C122" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="H122" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C123" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="H123" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C124" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>152</v>
       </c>
       <c r="H124" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C125" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="H125" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C126" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>154</v>
       </c>
       <c r="H126" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C127" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>155</v>
       </c>
       <c r="H127" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C128" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>156</v>
       </c>
       <c r="H128" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C129" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
       <c r="H129" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C130" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>158</v>
       </c>
       <c r="H130" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C131" s="23">
-        <f t="shared" ref="C131:C193" si="4">C130+1</f>
+        <f t="shared" ref="C131:C193" si="5">C130+1</f>
         <v>159</v>
       </c>
       <c r="H131" s="22" t="str">
-        <f t="shared" ref="H131:H194" si="5">IF(F131+G131&gt;0,G131/(G131+F131),"")</f>
+        <f t="shared" ref="H131:H194" si="6">IF(F131+G131&gt;0,G131/(G131+F131),"")</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C132" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="H132" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C133" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="H133" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C134" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="H134" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C135" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>163</v>
       </c>
       <c r="H135" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C136" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>164</v>
       </c>
       <c r="H136" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C137" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="H137" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C138" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>166</v>
       </c>
       <c r="H138" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C139" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>167</v>
       </c>
       <c r="H139" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C140" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="H140" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C141" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>169</v>
       </c>
       <c r="H141" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C142" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="H142" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C143" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>171</v>
       </c>
       <c r="H143" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C144" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>172</v>
       </c>
       <c r="H144" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C145" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>173</v>
       </c>
       <c r="H145" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C146" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>174</v>
       </c>
       <c r="H146" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C147" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="H147" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C148" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176</v>
       </c>
       <c r="H148" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C149" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="H149" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C150" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="H150" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C151" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>179</v>
       </c>
       <c r="H151" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C152" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="H152" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C153" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>181</v>
       </c>
       <c r="H153" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C154" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>182</v>
       </c>
       <c r="H154" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C155" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>183</v>
       </c>
       <c r="H155" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C156" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>184</v>
       </c>
       <c r="H156" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C157" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>185</v>
       </c>
       <c r="H157" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C158" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>186</v>
       </c>
       <c r="H158" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C159" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>187</v>
       </c>
       <c r="H159" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C160" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>188</v>
       </c>
       <c r="H160" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C161" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="H161" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C162" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="H162" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C163" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="H163" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C164" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="H164" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C165" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>193</v>
       </c>
       <c r="H165" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C166" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>194</v>
       </c>
       <c r="H166" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C167" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="H167" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C168" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>196</v>
       </c>
       <c r="H168" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C169" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>197</v>
       </c>
       <c r="H169" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C170" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>198</v>
       </c>
       <c r="H170" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C171" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>199</v>
       </c>
       <c r="H171" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="172" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C172" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="H172" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C173" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>201</v>
       </c>
       <c r="H173" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C174" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>202</v>
       </c>
       <c r="H174" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C175" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>203</v>
       </c>
       <c r="H175" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C176" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="H176" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C177" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>205</v>
       </c>
       <c r="H177" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C178" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>206</v>
       </c>
       <c r="H178" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C179" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>207</v>
       </c>
       <c r="H179" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C180" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>208</v>
       </c>
       <c r="H180" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C181" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>209</v>
       </c>
       <c r="H181" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C182" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
       <c r="H182" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C183" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>211</v>
       </c>
       <c r="H183" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C184" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>212</v>
       </c>
       <c r="H184" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C185" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>213</v>
       </c>
       <c r="H185" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C186" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>214</v>
       </c>
       <c r="H186" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C187" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>215</v>
       </c>
       <c r="H187" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C188" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>216</v>
       </c>
       <c r="H188" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C189" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>217</v>
       </c>
       <c r="H189" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C190" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>218</v>
       </c>
       <c r="H190" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C191" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>219</v>
       </c>
       <c r="H191" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C192" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>220</v>
       </c>
       <c r="H192" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C193" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>221</v>
       </c>
       <c r="H193" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H194" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H195" s="22" t="str">
-        <f t="shared" ref="H195:H258" si="6">IF(F195+G195&gt;0,G195/(G195+F195),"")</f>
+        <f t="shared" ref="H195:H258" si="7">IF(F195+G195&gt;0,G195/(G195+F195),"")</f>
         <v/>
       </c>
     </row>
     <row r="196" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H196" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H197" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H198" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H199" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H200" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H201" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H202" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H203" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H204" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H205" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H206" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H207" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H208" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H209" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H210" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H211" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H212" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H213" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H214" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H215" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H216" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H217" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H218" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H219" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H220" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H221" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H222" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H223" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H224" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H225" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H226" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H227" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H228" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H229" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H230" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H231" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H232" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H233" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H234" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H235" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H236" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H237" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H238" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H239" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H240" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H241" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H242" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H243" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H244" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H245" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H246" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H247" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H248" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H249" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H250" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H251" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H252" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H253" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H254" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H255" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H256" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H257" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H258" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H259" s="22" t="str">
-        <f t="shared" ref="H259:H280" si="7">IF(F259+G259&gt;0,G259/(G259+F259),"")</f>
+        <f t="shared" ref="H259:H280" si="8">IF(F259+G259&gt;0,G259/(G259+F259),"")</f>
         <v/>
       </c>
     </row>
     <row r="260" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H260" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H261" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H262" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H263" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H264" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H265" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H266" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="267" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H267" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="268" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H268" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="269" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H269" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="270" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H270" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="271" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H271" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="272" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H272" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="273" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H273" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="274" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H274" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="275" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H275" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="276" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H276" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="277" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H277" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="278" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H278" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="279" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H279" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="280" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H280" s="22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="281" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H281" s="24" t="str">
-        <f t="shared" ref="H281:H302" si="8">IF(F281&gt;0,G281/(G281+F281),"")</f>
+        <f t="shared" ref="H281:H302" si="9">IF(F281&gt;0,G281/(G281+F281),"")</f>
         <v/>
       </c>
     </row>
     <row r="282" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H282" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="283" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H283" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="284" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H284" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="285" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H285" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="286" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H286" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="287" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H287" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="288" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H288" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="289" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H289" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="290" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H290" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="291" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H291" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="292" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H292" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="293" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H293" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="294" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H294" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="295" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H295" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="296" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H296" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="297" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H297" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="298" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H298" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="299" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H299" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="300" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H300" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="301" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H301" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
     <row r="302" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H302" s="24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -10290,9 +10479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10374,45 +10563,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>16.25</v>
+        <v>28.75</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>16.5</v>
+        <v>2</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>0.49618320610687022</v>
+        <v>0.93495934959349591</v>
       </c>
       <c r="K2" s="16">
         <v>42604</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42654</v>
+        <v>42666</v>
       </c>
       <c r="M2" s="16">
         <v>42667</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>0.79365079365079361</v>
+        <v>0.98412698412698407</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.29746758754392338</v>
+        <v>-4.9167634533488158E-2</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-18.740458015267173</v>
+        <v>-3.097560975609754</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -10506,15 +10695,15 @@
       </c>
       <c r="B8" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A8)</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C8" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A8)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -10523,15 +10712,15 @@
       </c>
       <c r="B9" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A9)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A9)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -10540,15 +10729,15 @@
       </c>
       <c r="B10" s="5">
         <f>SUMIFS('Phase 2 Tasks'!G:G,'Phase 2 Tasks'!D:D,A10)</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="C10" s="5">
         <f>SUMIFS('Phase 2 Tasks'!F:F,'Phase 2 Tasks'!D:D,A10)</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -12258,7 +12447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12300,20 +12489,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="21">
         <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C2)</f>
@@ -12326,20 +12515,20 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C66" si="0">C2+1</f>
         <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" s="23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G3" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C3)</f>
@@ -12352,14 +12541,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="23">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="23">
         <v>4</v>
@@ -12378,14 +12567,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="23">
         <v>4</v>
@@ -12404,14 +12593,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="23">
         <v>6</v>
@@ -12430,14 +12619,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="23">
         <v>1</v>
@@ -12456,7 +12645,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="23">
         <f t="shared" si="0"/>
@@ -15188,7 +15377,7 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
@@ -15199,18 +15388,18 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42654</v>
+        <v>42666</v>
       </c>
       <c r="M2" s="16">
         <v>42713</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>-13</v>
+        <v>-1</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">IF(N2&gt;0,N2/(N2+O2),0)</f>
@@ -15227,7 +15416,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A3)</f>
@@ -15235,7 +15424,7 @@
       </c>
       <c r="C3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A3)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D65" si="0">IF(C3+B3&gt;0,B3/(B3+C3),"")</f>
@@ -15244,7 +15433,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A4)</f>
@@ -15252,7 +15441,7 @@
       </c>
       <c r="C4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A4)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
@@ -15261,7 +15450,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A5)</f>
@@ -15278,7 +15467,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A6)</f>
@@ -15295,7 +15484,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A7)</f>
@@ -17032,7 +17221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -17046,17 +17235,17 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="E1" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
       <c r="I1" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" s="36"/>
       <c r="K1" s="37"/>
@@ -17064,7 +17253,7 @@
         <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>51</v>
@@ -17073,7 +17262,7 @@
         <v>48</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>52</v>
@@ -17121,33 +17310,33 @@
       </c>
       <c r="N2" s="17">
         <f ca="1">TODAY()</f>
-        <v>42654</v>
+        <v>42666</v>
       </c>
       <c r="O2" s="17">
         <v>42713</v>
       </c>
       <c r="P2" s="5">
         <f ca="1">N2-M2</f>
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="Q2" s="5">
         <v>25</v>
       </c>
       <c r="R2" s="5">
         <f ca="1">O2-N2</f>
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="S2" s="28">
         <f ca="1">IF(P2&gt;0,(P2-Q2)/(P2+R2-Q2),0)</f>
-        <v>0.63354037267080743</v>
+        <v>0.70807453416149069</v>
       </c>
       <c r="T2" s="6">
         <f ca="1">G10-S2</f>
-        <v>-0.18592132505175979</v>
+        <v>-0.12525244827192017</v>
       </c>
       <c r="U2" s="30">
         <f ca="1">T2*(P2+R2-Q2)</f>
-        <v>-29.933333333333326</v>
+        <v>-20.165644171779146</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17165,15 +17354,15 @@
       </c>
       <c r="E3" s="31">
         <f>'Phase 2 Portfolio'!G2</f>
-        <v>16.25</v>
+        <v>28.75</v>
       </c>
       <c r="F3" s="32">
         <f>'Phase 2 Portfolio'!H2</f>
-        <v>16.5</v>
+        <v>2</v>
       </c>
       <c r="G3" s="33">
         <f>'Phase 2 Portfolio'!I2</f>
-        <v>0.49618320610687022</v>
+        <v>0.93495934959349591</v>
       </c>
       <c r="I3" s="31">
         <f>'Phase 3 Portfolio'!G2</f>
@@ -17181,7 +17370,7 @@
       </c>
       <c r="J3" s="32">
         <f>'Phase 3 Portfolio'!H2</f>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K3" s="33">
         <f>'Phase 3 Portfolio'!I2</f>
@@ -17191,7 +17380,7 @@
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
@@ -17210,15 +17399,15 @@
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="31">
         <f>A3+E3+I3</f>
-        <v>58.75</v>
+        <v>71.25</v>
       </c>
       <c r="F10" s="32">
         <f>B3+F3+J3</f>
-        <v>72.5</v>
+        <v>51</v>
       </c>
       <c r="G10" s="33">
         <f>E10/(E10+F10)</f>
-        <v>0.44761904761904764</v>
+        <v>0.58282208588957052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Document Templates and more code
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Time Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -359,12 +359,6 @@
     <t>Peform Integration Testing</t>
   </si>
   <si>
-    <t>Write User Manual</t>
-  </si>
-  <si>
-    <t>Project Evaluation</t>
-  </si>
-  <si>
     <t>Phase 1</t>
   </si>
   <si>
@@ -519,6 +513,30 @@
   </si>
   <si>
     <t>Prep and send out inspection and review Blakes</t>
+  </si>
+  <si>
+    <t>Finish Assesment</t>
+  </si>
+  <si>
+    <t>Assesment Evaluation</t>
+  </si>
+  <si>
+    <t>Set Up User Manual</t>
+  </si>
+  <si>
+    <t>Finish User Manual</t>
+  </si>
+  <si>
+    <t>Set Up Project Evaluation</t>
+  </si>
+  <si>
+    <t>Finish Evaluation</t>
+  </si>
+  <si>
+    <t>Set Up Assesment Evaluation</t>
+  </si>
+  <si>
+    <t>Write API</t>
   </si>
 </sst>
 </file>
@@ -1320,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA62" sqref="AA62"/>
+      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1909,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1905,7 +1923,7 @@
         <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1937,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +1973,7 @@
         <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +1987,7 @@
         <v>32</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1983,7 +2001,7 @@
         <v>42</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1997,7 +2015,7 @@
         <v>43</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2011,7 +2029,7 @@
         <v>43</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2025,7 +2043,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,7 +2057,7 @@
         <v>33</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,7 +2071,7 @@
         <v>33</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,7 +2085,7 @@
         <v>45</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +2110,7 @@
         <v>46</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,7 +2124,7 @@
         <v>46</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2149,7 @@
         <v>48</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2145,7 +2163,7 @@
         <v>35</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,7 +2177,7 @@
         <v>51</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,7 +2191,7 @@
         <v>52</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,7 +2219,7 @@
         <v>54</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2215,7 +2233,7 @@
         <v>55</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,7 +2247,7 @@
         <v>56</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2243,7 +2261,7 @@
         <v>57</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,7 +2275,7 @@
         <v>38</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,7 +2289,7 @@
         <v>38</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,7 +2303,7 @@
         <v>38</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,7 +2317,7 @@
         <v>57</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2313,7 +2331,7 @@
         <v>40</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2429,7 +2447,76 @@
         <v>79</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="17">
+        <v>42697</v>
+      </c>
+      <c r="B84" s="23">
+        <v>3</v>
+      </c>
+      <c r="C84" s="23">
+        <v>70</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="17">
+        <v>42698</v>
+      </c>
+      <c r="B85" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C85" s="23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="17">
+        <v>42699</v>
+      </c>
+      <c r="B86" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C86" s="23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="17">
+        <v>42699</v>
+      </c>
+      <c r="B87" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C87" s="23">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="17">
+        <v>42702</v>
+      </c>
+      <c r="B88" s="23">
+        <v>2</v>
+      </c>
+      <c r="C88" s="23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="17">
+        <v>42704</v>
+      </c>
+      <c r="B89" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C89" s="23">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5676,14 +5763,14 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42697</v>
+        <v>42704</v>
       </c>
       <c r="M2" s="16">
         <v>42580</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">IF(M2-L2&gt;0,M2-L2,0)</f>
@@ -7634,7 +7721,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>38</v>
@@ -7683,7 +7770,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>38</v>
@@ -7729,7 +7816,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C9" s="23">
         <f t="shared" si="0"/>
@@ -7830,7 +7917,7 @@
         <v>98</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
@@ -7856,7 +7943,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>38</v>
@@ -7885,7 +7972,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>38</v>
@@ -7914,7 +8001,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>38</v>
@@ -7943,7 +8030,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>38</v>
@@ -7972,7 +8059,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>38</v>
@@ -8001,7 +8088,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>38</v>
@@ -8030,7 +8117,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>38</v>
@@ -8059,7 +8146,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>38</v>
@@ -8088,7 +8175,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>38</v>
@@ -8117,7 +8204,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>38</v>
@@ -8146,7 +8233,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>38</v>
@@ -8175,7 +8262,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>38</v>
@@ -8204,7 +8291,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>38</v>
@@ -8233,7 +8320,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>38</v>
@@ -8262,7 +8349,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>38</v>
@@ -8291,7 +8378,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>38</v>
@@ -10734,30 +10821,30 @@
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42697</v>
+        <v>42704</v>
       </c>
       <c r="M2" s="16">
         <v>42667</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>-30</v>
+        <v>-37</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">N2/(N2+O2)</f>
-        <v>1.4761904761904763</v>
+        <v>1.5873015873015872</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.47619047619047628</v>
+        <v>-0.58730158730158721</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-30.000000000000007</v>
+        <v>-36.999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -12603,7 +12690,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12647,7 +12734,9 @@
       <c r="A2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="C2" s="21">
         <v>70</v>
       </c>
@@ -12658,15 +12747,15 @@
         <v>4</v>
       </c>
       <c r="F2" s="21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C2)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" s="22">
         <f>IF(F2+G2&gt;0,G2/(G2+F2),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -12674,7 +12763,7 @@
         <v>104</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="23">
         <f t="shared" ref="C3:C66" si="0">C2+1</f>
@@ -12684,18 +12773,18 @@
         <v>100</v>
       </c>
       <c r="E3" s="23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C3)</f>
-        <v>14</v>
+        <v>17.5</v>
       </c>
       <c r="H3" s="22">
         <f t="shared" ref="H3:H66" si="1">IF(F3+G3&gt;0,G3/(G3+F3),"")</f>
-        <v>0.93333333333333335</v>
+        <v>0.89743589743589747</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -12710,10 +12799,10 @@
         <v>101</v>
       </c>
       <c r="E4" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C4)</f>
@@ -12736,10 +12825,10 @@
         <v>101</v>
       </c>
       <c r="E5" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C5)</f>
@@ -12752,7 +12841,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="0"/>
@@ -12762,10 +12851,10 @@
         <v>102</v>
       </c>
       <c r="E6" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C6)</f>
@@ -12778,7 +12867,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C7" s="23">
         <f t="shared" si="0"/>
@@ -12882,7 +12971,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="23">
         <f t="shared" si="0"/>
@@ -12907,73 +12996,142 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="C12" s="23">
         <f t="shared" si="0"/>
         <v>80</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="23">
+        <v>1</v>
+      </c>
+      <c r="F12" s="23">
+        <v>1</v>
       </c>
       <c r="G12" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H12" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="C13" s="23">
         <f t="shared" si="0"/>
         <v>81</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="23">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0</v>
       </c>
       <c r="G13" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C13)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="23">
+        <v>1</v>
+      </c>
+      <c r="F14" s="23">
         <v>0</v>
-      </c>
-      <c r="H13" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="23">
-        <f t="shared" si="0"/>
-        <v>82</v>
       </c>
       <c r="G14" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C14)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="23">
+        <v>1</v>
+      </c>
+      <c r="F15" s="23">
         <v>0</v>
-      </c>
-      <c r="H14" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="23">
-        <f t="shared" si="0"/>
-        <v>83</v>
       </c>
       <c r="G15" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C15)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="C16" s="23">
         <f t="shared" si="0"/>
         <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="23">
+        <v>1</v>
+      </c>
+      <c r="F16" s="23">
+        <v>1</v>
       </c>
       <c r="G16" s="21">
         <f>SUMIFS('Time Log'!B:B,'Time Log'!C:C,'Phase 3 Tasks'!C16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H16" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -15460,9 +15618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R288"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15544,45 +15702,45 @@
       </c>
       <c r="G2" s="5">
         <f>SUM(B:B)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(C:C)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I2" s="6">
         <f>IF(H2+G2&gt;0,G2/(G2+H2),"")</f>
-        <v>0.42105263157894735</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="K2" s="16">
         <v>42667</v>
       </c>
       <c r="L2" s="16">
         <f ca="1">TODAY()</f>
-        <v>42697</v>
+        <v>42704</v>
       </c>
       <c r="M2" s="16">
-        <v>42713</v>
+        <v>42716</v>
       </c>
       <c r="N2" s="5">
         <f ca="1">L2-K2</f>
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="O2" s="5">
         <f ca="1">M2-L2</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P2" s="28">
         <f ca="1">IF(N2&gt;0,N2/(N2+O2),0)</f>
-        <v>0.65217391304347827</v>
+        <v>0.75510204081632648</v>
       </c>
       <c r="Q2" s="6">
         <f ca="1">I2-P2</f>
-        <v>-0.23112128146453093</v>
+        <v>-0.13971742543171106</v>
       </c>
       <c r="R2" s="30">
         <f ca="1">Q2*(N2+O2)</f>
-        <v>-10.631578947368423</v>
+        <v>-6.8461538461538423</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -15591,15 +15749,15 @@
       </c>
       <c r="B3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A3)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D65" si="0">IF(C3+B3&gt;0,B3/(B3+C3),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -15608,15 +15766,15 @@
       </c>
       <c r="B4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A4)</f>
-        <v>14</v>
+        <v>17.5</v>
       </c>
       <c r="C4" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
+        <v>0.89743589743589747</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -15629,7 +15787,7 @@
       </c>
       <c r="C5" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A5)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
@@ -15642,15 +15800,15 @@
       </c>
       <c r="B6" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A6)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A6)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -15659,7 +15817,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A7)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="5">
         <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A7)</f>
@@ -15667,7 +15825,7 @@
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -15705,9 +15863,20 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="5">
+        <f>SUMIFS('Phase 3 Tasks'!G:G,'Phase 3 Tasks'!D:D,A10)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="5">
+        <f>SUMIFS('Phase 3 Tasks'!F:F,'Phase 3 Tasks'!D:D,A10)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" ref="D10" si="2">IF(C10+B10&gt;0,B10/(B10+C10),"")</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -16042,1339 +16211,1339 @@
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="11" t="str">
-        <f t="shared" ref="D66:D129" si="2">IF(C66+B66&gt;0,B66/(B66+C66),"")</f>
+        <f t="shared" ref="D66:D129" si="3">IF(C66+B66&gt;0,B66/(B66+C66),"")</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" s="11" t="str">
-        <f t="shared" ref="D130:D170" si="3">IF(C130+B130&gt;0,B130/(B130+C130),"")</f>
+        <f t="shared" ref="D130:D170" si="4">IF(C130+B130&gt;0,B130/(B130+C130),"")</f>
         <v/>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D155" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D156" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D157" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D158" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D159" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D160" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="161" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D161" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="162" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D162" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="163" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D163" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="164" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D164" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="165" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D165" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="166" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D166" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="167" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D167" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="168" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D168" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D169" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D170" s="11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="4" t="str">
-        <f t="shared" ref="D171:D234" si="4">IF(C171&gt;0,B171/(B171+C171),"")</f>
+        <f t="shared" ref="D171:D234" si="5">IF(C171&gt;0,B171/(B171+C171),"")</f>
         <v/>
       </c>
     </row>
     <row r="172" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D172" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="173" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D173" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="174" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D174" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="175" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D175" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="176" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D176" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="177" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D177" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="178" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D178" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="179" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D179" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="180" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D180" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="181" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D181" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="182" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D182" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="183" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D183" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="184" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D184" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="185" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D185" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="186" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D186" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="187" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D187" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="188" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D188" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="189" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D189" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="190" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D190" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="191" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D191" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="192" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D192" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="193" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D193" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="194" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D194" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="195" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D195" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="196" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D196" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D197" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="198" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D198" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="199" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D199" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="200" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D200" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="201" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D201" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="202" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D202" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="203" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D203" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="204" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D204" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="205" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D205" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D206" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D207" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D208" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D209" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="210" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D210" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="211" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D211" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="212" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D212" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="213" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D213" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="214" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D214" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="215" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D215" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="216" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D216" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="217" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D217" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="218" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D218" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="219" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D219" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="220" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D220" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="221" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D221" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="222" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D222" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="223" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D223" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="224" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D224" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="225" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D225" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="226" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D226" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="227" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D227" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="228" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D228" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="229" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D229" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="230" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D230" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="231" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D231" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="232" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D232" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="233" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D233" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D234" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D235" s="4" t="str">
-        <f t="shared" ref="D235:D288" si="5">IF(C235&gt;0,B235/(B235+C235),"")</f>
+        <f t="shared" ref="D235:D288" si="6">IF(C235&gt;0,B235/(B235+C235),"")</f>
         <v/>
       </c>
     </row>
     <row r="236" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D236" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="237" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D237" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="238" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D238" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="239" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D239" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="240" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D240" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="241" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D241" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="242" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D242" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="243" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D243" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="244" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D244" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="245" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D245" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="246" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D246" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="247" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D247" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="248" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D248" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D249" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="250" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D250" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="251" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D251" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="252" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D252" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="253" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D253" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="254" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D254" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="255" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D255" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="256" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D256" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="257" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D257" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="258" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D258" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="259" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D259" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="260" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D260" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D261" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="262" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D262" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="263" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D263" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="264" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D264" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="265" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D265" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="266" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D266" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="267" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D267" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="268" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D268" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="269" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D269" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="270" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D270" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="271" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D271" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="272" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D272" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="274" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D274" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="275" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D275" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="276" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D276" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="277" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D277" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="278" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D278" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="279" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D279" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="280" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D280" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="281" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D281" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="282" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D282" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="283" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D283" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="284" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D284" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="285" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D285" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="286" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D286" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="287" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D287" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="288" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D288" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17404,7 +17573,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17417,17 +17586,17 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="E1" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
       <c r="I1" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J1" s="36"/>
       <c r="K1" s="37"/>
@@ -17435,7 +17604,7 @@
         <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>51</v>
@@ -17444,7 +17613,7 @@
         <v>48</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>52</v>
@@ -17492,33 +17661,33 @@
       </c>
       <c r="N2" s="17">
         <f ca="1">TODAY()</f>
-        <v>42697</v>
+        <v>42704</v>
       </c>
       <c r="O2" s="17">
-        <v>42713</v>
+        <v>42716</v>
       </c>
       <c r="P2" s="5">
         <f ca="1">N2-M2</f>
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="Q2" s="5">
         <v>25</v>
       </c>
       <c r="R2" s="5">
         <f ca="1">O2-N2</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="S2" s="28">
         <f ca="1">IF(P2&gt;0,(P2-Q2)/(P2+R2-Q2),0)</f>
-        <v>0.90062111801242239</v>
+        <v>0.92682926829268297</v>
       </c>
       <c r="T2" s="6">
         <f ca="1">G10-S2</f>
-        <v>-9.8819316210620567E-2</v>
+        <v>-6.075783972125437E-2</v>
       </c>
       <c r="U2" s="30">
         <f ca="1">T2*(P2+R2-Q2)</f>
-        <v>-15.909909909909912</v>
+        <v>-9.9642857142857171</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17548,21 +17717,21 @@
       </c>
       <c r="I3" s="31">
         <f>'Phase 3 Portfolio'!G2</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J3" s="32">
         <f>'Phase 3 Portfolio'!H2</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K3" s="33">
         <f>'Phase 3 Portfolio'!I2</f>
-        <v>0.42105263157894735</v>
+        <v>0.61538461538461542</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
@@ -17581,15 +17750,15 @@
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="31">
         <f>A3+E3+I3</f>
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F10" s="32">
         <f>B3+F3+J3</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G10" s="33">
         <f>E10/(E10+F10)</f>
-        <v>0.80180180180180183</v>
+        <v>0.8660714285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>